<commit_message>
looting system + upgrading changes
+ Crates to loot
+ functions to loot crates
+ added calculations to math wether upgrades can be bought
+ added images for the wire and glass upgrades
</commit_message>
<xml_diff>
--- a/App/Maps/SP3_Map.xlsx
+++ b/App/Maps/SP3_Map.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3694abd74283ce8b/Documents/GitHub/Studio_Project3/App/Maps/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kohli\Documents\GitHub\Studio_Project3\App\Maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="283" documentId="8_{83B8CE0D-2E42-4F4D-9C73-8BBFEA985F7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1443C53B-6E1A-44CC-AF2A-DE07A492AAB4}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65ACA275-12AF-43A0-B1BA-F87C75EA6971}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9E6FBB19-5B0A-45BE-B993-369F54EB6B5F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9E6FBB19-5B0A-45BE-B993-369F54EB6B5F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -472,8 +472,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93CFF945-3A7D-4A58-BBFC-9631FB7B426B}">
   <dimension ref="A1:EU150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Z63" sqref="Z63"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AN56" sqref="AN56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>